<commit_message>
updates validators for new checks
- differentiate sncu/rch
- no need for list in mandatory columns
- bring a structure to validators by using run instead of validate
</commit_message>
<xml_diff>
--- a/custom/samveg/tests/case_importer/data/case_upload.xlsx
+++ b/custom/samveg/tests/case_importer/data/case_upload.xlsx
@@ -20,7 +20,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+  <si>
+    <t xml:space="preserve">Rch_id</t>
+  </si>
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -129,27 +132,30 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>2</v>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
       </c>
-      <c r="B2" s="1" t="n">
+      <c r="C2" s="1" t="n">
         <v>2</v>
       </c>
     </row>

</xml_diff>